<commit_message>
Add comment to  PreQual-Table.xlsx
Add comment to  PreQual-Table.xlsx
</commit_message>
<xml_diff>
--- a/Prequal Table Schema - 21'03.xlsx
+++ b/Prequal Table Schema - 21'03.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git-hub.com Clone\Springboot-Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB4AE74-8291-4C4D-91D2-8D33FBEB8405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5544" yWindow="108" windowWidth="17280" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,14 +24,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="3">
+  <si>
+    <t xml:space="preserve">[Definition] 
+[Range/List] 
+[Example]
+[Reference] </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STATUS_FAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAC_MATCH_RESULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,11 +82,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +369,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="9" style="2"/>
+    <col min="5" max="5" width="39.5" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add SQL Script Template v1-21'03.txt
Add 'SQL Script Template v1-21'03.txt'
</commit_message>
<xml_diff>
--- a/Prequal Table Schema - 21'03.xlsx
+++ b/Prequal Table Schema - 21'03.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git-hub.com Clone\Springboot-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB4AE74-8291-4C4D-91D2-8D33FBEB8405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB69A9C-9501-4048-A145-31B9CD07C250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5544" yWindow="108" windowWidth="17280" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4344" yWindow="1032" windowWidth="17280" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
Update Prequal Table Schema - 21'03.xlsx
</commit_message>
<xml_diff>
--- a/Prequal Table Schema - 21'03.xlsx
+++ b/Prequal Table Schema - 21'03.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git-hub.com Clone\Springboot-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4B1E2B-23C7-45DF-BBB2-FB6C78F16DB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0BBE4-1861-4457-A32B-A238E4E3D11D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="144" windowWidth="22488" windowHeight="11808" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="14532" windowHeight="11808" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="RAWMAT_PRE_BATCH_STATUS" sheetId="2" r:id="rId2"/>
-    <sheet name="工作表1" sheetId="4" r:id="rId3"/>
-    <sheet name="RAWMAT_MONITOR_RESULT" sheetId="3" r:id="rId4"/>
+    <sheet name="RAWMAT_PRE_BATCH_STATUS (2)" sheetId="5" r:id="rId2"/>
+    <sheet name="RAWMAT_PRE_BATCH_STATUS" sheetId="2" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="4" r:id="rId4"/>
+    <sheet name="RAWMAT_MONITOR_RESULT" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="179">
   <si>
     <t xml:space="preserve">[Definition] 
 [Range/List] 
@@ -554,6 +555,40 @@
   </si>
   <si>
     <t>FAC_MATCH_STATUS;</t>
+  </si>
+  <si>
+    <t>MONITOR_SEC_NAME VARCHAR2(1024 BYTE),</t>
+  </si>
+  <si>
+    <t>MON_DEPT_NAME VARCHAR2(65 BYTE),</t>
+  </si>
+  <si>
+    <t>IS_ON_TOOL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IS_USED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PKG_STATUS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PKG_RESULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4 CHAR)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RISK_TIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CYCLE_TIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -576,12 +611,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -596,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -604,6 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -966,6 +1008,973 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289B50DE-FB3E-494D-AC84-D3DB8BA01845}">
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F67" si="0">CONCATENATE(B3," ",C3, D3, IF(ISBLANK(E3), "", CONCATENATE(" ",E3)), ",")</f>
+        <v>MAT_NO VARCHAR2(80 CHAR),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>BATCH_ID VARCHAR2(80 CHAR),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="str">
+        <f>CONCATENATE(B5," ",C5, D5, IF(ISBLANK(E5), "", CONCATENATE(" ",E5)), ",")</f>
+        <v>FAB_PLANT_CD VARCHAR2(10 CHAR),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6" si="1">CONCATENATE(B6," ",C6, D6, IF(ISBLANK(E6), "", CONCATENATE(" ",E6)), ",")</f>
+        <v>MAT_NAME VARCHAR2(80 CHAR) DEFAULT '0',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="str">
+        <f>CONCATENATE(B23," ",C23, D23, IF(ISBLANK(E23), "", CONCATENATE(" ",E23)), ",")</f>
+        <v>CASE_ID NUMBER(10,0),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="str">
+        <f>CONCATENATE(B24," ",C24, D24, IF(ISBLANK(E24), "", CONCATENATE(" ",E24)), ",")</f>
+        <v>FAB_NAME VARCHAR2(10 CHAR),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="str">
+        <f>CONCATENATE(B25," ",C25, D25, IF(ISBLANK(E25), "", CONCATENATE(" ",E25)), ",")</f>
+        <v>FAB_CD VARCHAR2(2 CHAR),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="str">
+        <f>CONCATENATE(B26," ",C26, D26, IF(ISBLANK(E26), "", CONCATENATE(" ",E26)), ",")</f>
+        <v>TOOL_ID VARCHAR2(2048 BYTE),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" t="str">
+        <f>CONCATENATE(B27," ",C27, D27, IF(ISBLANK(E27), "", CONCATENATE(" ",E27)), ",")</f>
+        <v>LOOP_ID VARCHAR2(40 BYTE),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="str">
+        <f>CONCATENATE(B28," ",C28, D28, IF(ISBLANK(E28), "", CONCATENATE(" ",E28)), ",")</f>
+        <v>PORT VARCHAR2(20 CHAR),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>CONTR_ID VARCHAR2(80 CHAR) DEFAULT '&lt;N/A&gt;',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>MAT_CHANGE_DT DATE NOT NULL,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>RMNDR_AMOUNT FLOAT(126) DEFAULT '0',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>CASE_STATUS NUMBER(10,0) DEFAULT '0',</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>LAST_CHK_DT DATE DEFAULT *,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>CONFIRM_LOT_COUNT NUMBER(10,0) DEFAULT '0',</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>LEADING_LOT VARCHAR2(20 CHAR),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>CONFIRM_LOT_LIST VARCHAR2(400 CHAR),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>STEP_ID VARCHAR2(50 CHAR),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>STEP_ID_LIST VARCHAR2(200 CHAR) ,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>IS_PIRUN VARCHAR2(1 CHAR) DEFAULT 'N',</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>RMNDR_CHK_TIME NUMBER(10,0) DEFAULT '0',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>PART_ID VARCHAR2(32 CHAR),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>CHECK_TYPE VARCHAR2(8 CHAR),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>PHASE_ID VARCHAR2(8 CHAR),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE_SYSTEM VARCHAR2(40 CHAR),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>LATEST_CASE NUMBER(10,0) DEFAULT '0',</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>REPORT_OBJECT_ID VARCHAR2(100 CHAR),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>MAIL_LIST VARCHAR2(2048 CHAR),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>MONITOR_SECTION VARCHAR2(512 CHAR),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>PREQ_RESULT VARCHAR2(10 CHAR),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>SPC_MATCH_STATUS VARCHAR2(4 CHAR),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>PREQ_USER VARCHAR2(15 CHAR),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>VENDOR_CD VARCHAR2(20 CHAR),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>65</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>PREQ_FORM_NO VARCHAR2(60 CHAR),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>CONFIRM_LOT_TOOL VARCHAR2(34 CHAR),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>FAC_TOOL_TYPE VARCHAR2(10 BYTE),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>TANK_ID VARCHAR2(20 BYTE),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>TANK_SWITCH_DT DATE,</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>MAT_USED_DT DATE,</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>CASE_STATUS_DEFECT NUMBER(10,0),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>DEFECT_MATCH_STATUS VARCHAR2(4 BYTE),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>IS_NEW_BATCH VARCHAR2(1 BYTE),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>108</v>
+      </c>
+      <c r="B65" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>CASE_CLOSE_TIME DATE,</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>CASE_STATUS_FAC NUMBER(10,0),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="0"/>
+        <v>FAC_MATCH_STATUS VARCHAR2(4 BYTE),</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FBBE9DB-60EF-4DAB-BB40-EDD012F61309}">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -1850,7 +2859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CA4860-E5F4-454D-8E01-6AB1AC196CDA}">
   <dimension ref="D2:G49"/>
   <sheetViews>
@@ -2544,11 +3553,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B7C8A6-4C4D-4D03-81EE-AE1277ABDA4C}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:J18"/>
     </sheetView>
   </sheetViews>

</xml_diff>